<commit_message>
cambiosd e estlos blanco y timeline
</commit_message>
<xml_diff>
--- a/public/data/DASHBOARD_PORTAFOLIO.xlsx
+++ b/public/data/DASHBOARD_PORTAFOLIO.xlsx
@@ -8,21 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VERYTEL\DESARROLLOS\portfolio-dashboard\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34025D05-997B-4259-8BEC-C3FCBBE8FC4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4F986C-BAD4-4C75-958B-B0426AE917B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard_Resumen" sheetId="1" r:id="rId1"/>
     <sheet name="Recursos" sheetId="3" r:id="rId2"/>
     <sheet name="Proyectos" sheetId="2" r:id="rId3"/>
-    <sheet name="Horas" sheetId="9" r:id="rId4"/>
-    <sheet name="Matriz_Horas" sheetId="4" r:id="rId5"/>
-    <sheet name="Tareas" sheetId="5" r:id="rId6"/>
-    <sheet name="Solapamientos" sheetId="6" r:id="rId7"/>
-    <sheet name="Timeline" sheetId="7" r:id="rId8"/>
-    <sheet name="Metricas_Graficos" sheetId="8" r:id="rId9"/>
+    <sheet name="Matriz_Horas" sheetId="4" r:id="rId4"/>
+    <sheet name="Tareas" sheetId="5" r:id="rId5"/>
+    <sheet name="Solapamientos" sheetId="6" r:id="rId6"/>
+    <sheet name="Timeline" sheetId="7" r:id="rId7"/>
+    <sheet name="Metricas_Graficos" sheetId="8" r:id="rId8"/>
+    <sheet name="Horas" sheetId="9" r:id="rId9"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Timeline!$A$1:$I$104</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -41,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1600" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1598" uniqueCount="378">
   <si>
     <t>DASHBOARD GERENCIAL - ANÁLISIS DE PORTAFOLIO</t>
   </si>
@@ -1159,9 +1162,6 @@
     <t>Sem 1</t>
   </si>
   <si>
-    <t>Juan David Sanchez</t>
-  </si>
-  <si>
     <t>total horas</t>
   </si>
   <si>
@@ -1172,6 +1172,12 @@
   </si>
   <si>
     <t>Recurso sin IA</t>
+  </si>
+  <si>
+    <t>XTAM CÁMARA</t>
+  </si>
+  <si>
+    <t>XTAM CÁMARAS</t>
   </si>
 </sst>
 </file>
@@ -1572,7 +1578,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1763,7 +1769,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2096,7 +2102,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2165,7 +2171,7 @@
         <v>48</v>
       </c>
       <c r="J2" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -2398,579 +2404,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893D026F-294B-4AEA-8E08-449915C9D86F}">
-  <dimension ref="A1:S11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S18" sqref="K18:S24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="8" width="0" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="30.7109375" customWidth="1"/>
-    <col min="12" max="18" width="0" hidden="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>375</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>368</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>369</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>370</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>371</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>368</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>369</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>370</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>374</v>
-      </c>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5" t="s">
-        <v>376</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>368</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>369</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>370</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>371</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>368</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>369</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>370</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B2">
-        <v>60</v>
-      </c>
-      <c r="C2">
-        <v>50</v>
-      </c>
-      <c r="D2">
-        <v>50</v>
-      </c>
-      <c r="E2">
-        <v>50</v>
-      </c>
-      <c r="F2">
-        <v>60</v>
-      </c>
-      <c r="G2">
-        <v>60</v>
-      </c>
-      <c r="H2">
-        <v>60</v>
-      </c>
-      <c r="I2" s="5">
-        <f t="shared" ref="I2:I8" si="0">SUM(B2:H2)</f>
-        <v>390</v>
-      </c>
-      <c r="K2" t="s">
-        <v>75</v>
-      </c>
-      <c r="L2">
-        <v>40</v>
-      </c>
-      <c r="M2">
-        <v>32</v>
-      </c>
-      <c r="N2">
-        <v>32</v>
-      </c>
-      <c r="O2">
-        <v>32</v>
-      </c>
-      <c r="P2">
-        <v>40</v>
-      </c>
-      <c r="Q2">
-        <v>40</v>
-      </c>
-      <c r="R2">
-        <v>40</v>
-      </c>
-      <c r="S2" s="5">
-        <f t="shared" ref="S2:S8" si="1">SUM(L2:R2)</f>
-        <v>256</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3">
-        <v>60</v>
-      </c>
-      <c r="C3">
-        <v>50</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>60</v>
-      </c>
-      <c r="H3">
-        <v>60</v>
-      </c>
-      <c r="I3" s="5">
-        <f t="shared" si="0"/>
-        <v>230</v>
-      </c>
-      <c r="K3" t="s">
-        <v>71</v>
-      </c>
-      <c r="L3">
-        <v>40</v>
-      </c>
-      <c r="M3">
-        <v>32</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>40</v>
-      </c>
-      <c r="R3">
-        <v>40</v>
-      </c>
-      <c r="S3" s="5">
-        <f t="shared" si="1"/>
-        <v>152</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4">
-        <v>60</v>
-      </c>
-      <c r="C4">
-        <v>50</v>
-      </c>
-      <c r="D4">
-        <v>50</v>
-      </c>
-      <c r="E4">
-        <v>50</v>
-      </c>
-      <c r="F4">
-        <v>60</v>
-      </c>
-      <c r="G4">
-        <v>60</v>
-      </c>
-      <c r="H4">
-        <v>60</v>
-      </c>
-      <c r="I4" s="5">
-        <f t="shared" si="0"/>
-        <v>390</v>
-      </c>
-      <c r="K4" t="s">
-        <v>74</v>
-      </c>
-      <c r="L4">
-        <v>40</v>
-      </c>
-      <c r="M4">
-        <v>32</v>
-      </c>
-      <c r="N4">
-        <v>32</v>
-      </c>
-      <c r="O4">
-        <v>32</v>
-      </c>
-      <c r="P4">
-        <v>40</v>
-      </c>
-      <c r="Q4">
-        <v>40</v>
-      </c>
-      <c r="R4">
-        <v>40</v>
-      </c>
-      <c r="S4" s="5">
-        <f t="shared" si="1"/>
-        <v>256</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B5">
-        <v>60</v>
-      </c>
-      <c r="C5">
-        <v>50</v>
-      </c>
-      <c r="D5">
-        <v>50</v>
-      </c>
-      <c r="E5">
-        <v>50</v>
-      </c>
-      <c r="F5">
-        <v>60</v>
-      </c>
-      <c r="G5">
-        <v>60</v>
-      </c>
-      <c r="H5">
-        <v>60</v>
-      </c>
-      <c r="I5" s="5">
-        <f t="shared" si="0"/>
-        <v>390</v>
-      </c>
-      <c r="K5" t="s">
-        <v>79</v>
-      </c>
-      <c r="L5">
-        <v>40</v>
-      </c>
-      <c r="M5">
-        <v>32</v>
-      </c>
-      <c r="N5">
-        <v>32</v>
-      </c>
-      <c r="O5">
-        <v>32</v>
-      </c>
-      <c r="P5">
-        <v>40</v>
-      </c>
-      <c r="Q5">
-        <v>40</v>
-      </c>
-      <c r="R5">
-        <v>40</v>
-      </c>
-      <c r="S5" s="5">
-        <f t="shared" si="1"/>
-        <v>256</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>372</v>
-      </c>
-      <c r="B6">
-        <v>60</v>
-      </c>
-      <c r="C6">
-        <v>50</v>
-      </c>
-      <c r="D6">
-        <v>50</v>
-      </c>
-      <c r="E6">
-        <v>50</v>
-      </c>
-      <c r="F6">
-        <v>60</v>
-      </c>
-      <c r="G6">
-        <v>60</v>
-      </c>
-      <c r="H6">
-        <v>60</v>
-      </c>
-      <c r="I6" s="5">
-        <f t="shared" si="0"/>
-        <v>390</v>
-      </c>
-      <c r="K6" t="s">
-        <v>372</v>
-      </c>
-      <c r="L6">
-        <v>40</v>
-      </c>
-      <c r="M6">
-        <v>32</v>
-      </c>
-      <c r="N6">
-        <v>32</v>
-      </c>
-      <c r="O6">
-        <v>32</v>
-      </c>
-      <c r="P6">
-        <v>40</v>
-      </c>
-      <c r="Q6">
-        <v>40</v>
-      </c>
-      <c r="R6">
-        <v>40</v>
-      </c>
-      <c r="S6" s="5">
-        <f t="shared" si="1"/>
-        <v>256</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B7">
-        <v>30</v>
-      </c>
-      <c r="C7">
-        <v>30</v>
-      </c>
-      <c r="D7">
-        <v>30</v>
-      </c>
-      <c r="E7">
-        <v>30</v>
-      </c>
-      <c r="F7">
-        <v>30</v>
-      </c>
-      <c r="G7">
-        <v>30</v>
-      </c>
-      <c r="H7">
-        <v>30</v>
-      </c>
-      <c r="I7" s="5">
-        <f t="shared" si="0"/>
-        <v>210</v>
-      </c>
-      <c r="K7" t="s">
-        <v>81</v>
-      </c>
-      <c r="L7">
-        <v>20</v>
-      </c>
-      <c r="M7">
-        <v>20</v>
-      </c>
-      <c r="N7">
-        <v>20</v>
-      </c>
-      <c r="O7">
-        <v>20</v>
-      </c>
-      <c r="P7">
-        <v>20</v>
-      </c>
-      <c r="Q7">
-        <v>20</v>
-      </c>
-      <c r="R7">
-        <v>20</v>
-      </c>
-      <c r="S7" s="5">
-        <f t="shared" si="1"/>
-        <v>140</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>82</v>
-      </c>
-      <c r="B8">
-        <v>60</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>50</v>
-      </c>
-      <c r="E8">
-        <v>50</v>
-      </c>
-      <c r="F8">
-        <v>60</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8" s="5">
-        <f t="shared" si="0"/>
-        <v>220</v>
-      </c>
-      <c r="K8" t="s">
-        <v>82</v>
-      </c>
-      <c r="L8">
-        <v>40</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>32</v>
-      </c>
-      <c r="O8">
-        <v>32</v>
-      </c>
-      <c r="P8">
-        <v>40</v>
-      </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-      <c r="S8" s="5">
-        <f t="shared" si="1"/>
-        <v>144</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>373</v>
-      </c>
-      <c r="B9">
-        <f>SUM(B2:B8)</f>
-        <v>390</v>
-      </c>
-      <c r="C9">
-        <f t="shared" ref="C9:H9" si="2">SUM(C2:C8)</f>
-        <v>280</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="2"/>
-        <v>280</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="2"/>
-        <v>280</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="2"/>
-        <v>330</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="2"/>
-        <v>330</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="2"/>
-        <v>330</v>
-      </c>
-      <c r="I9" s="5">
-        <f>SUM(B9:H9)</f>
-        <v>2220</v>
-      </c>
-      <c r="J9" s="5"/>
-      <c r="K9" t="s">
-        <v>373</v>
-      </c>
-      <c r="L9">
-        <f>SUM(L2:L8)</f>
-        <v>260</v>
-      </c>
-      <c r="M9">
-        <f t="shared" ref="M9" si="3">SUM(M2:M8)</f>
-        <v>180</v>
-      </c>
-      <c r="N9">
-        <f t="shared" ref="N9" si="4">SUM(N2:N8)</f>
-        <v>180</v>
-      </c>
-      <c r="O9">
-        <f t="shared" ref="O9" si="5">SUM(O2:O8)</f>
-        <v>180</v>
-      </c>
-      <c r="P9">
-        <f t="shared" ref="P9" si="6">SUM(P2:P8)</f>
-        <v>220</v>
-      </c>
-      <c r="Q9">
-        <f t="shared" ref="Q9" si="7">SUM(Q2:Q8)</f>
-        <v>220</v>
-      </c>
-      <c r="R9">
-        <f t="shared" ref="R9" si="8">SUM(R2:R8)</f>
-        <v>220</v>
-      </c>
-      <c r="S9" s="5">
-        <f>SUM(L9:R9)</f>
-        <v>1460</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="K11" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="12" width="18" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" customWidth="1"/>
+    <col min="2" max="10" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -2999,16 +2446,10 @@
         <v>83</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="L1" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -3019,7 +2460,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -3037,16 +2478,10 @@
         <v>27</v>
       </c>
       <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -3057,13 +2492,13 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>153</v>
+        <v>45</v>
       </c>
       <c r="G3">
         <v>36</v>
@@ -3075,16 +2510,10 @@
         <v>27</v>
       </c>
       <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
         <v>279</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -3113,16 +2542,10 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>9</v>
-      </c>
-      <c r="K4">
-        <v>9</v>
-      </c>
-      <c r="L4">
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -3130,7 +2553,7 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -3139,7 +2562,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -3151,16 +2574,10 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -3189,16 +2606,10 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
         <v>387</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -3206,7 +2617,7 @@
         <v>27</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -3215,7 +2626,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>130.5</v>
+        <v>80</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -3227,16 +2638,10 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
         <v>157.5</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -3265,16 +2670,10 @@
         <v>18</v>
       </c>
       <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
         <v>198</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -3303,50 +2702,67 @@
         <v>18</v>
       </c>
       <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
         <v>855</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>376</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B11" s="2">
         <v>360</v>
       </c>
-      <c r="C10" s="2">
-        <v>180</v>
-      </c>
-      <c r="D10" s="2">
-        <v>243</v>
-      </c>
-      <c r="E10" s="2">
+      <c r="C11" s="2">
+        <v>256</v>
+      </c>
+      <c r="D11" s="2">
+        <v>197</v>
+      </c>
+      <c r="E11" s="2">
         <v>360</v>
       </c>
-      <c r="F10" s="2">
-        <v>382.5</v>
-      </c>
-      <c r="G10" s="2">
+      <c r="F11" s="2">
+        <v>206</v>
+      </c>
+      <c r="G11" s="2">
         <v>234</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H11" s="2">
         <v>387</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I11" s="2">
         <v>90</v>
       </c>
-      <c r="J10" s="2">
-        <v>9</v>
-      </c>
-      <c r="K10" s="2">
-        <v>9</v>
-      </c>
-      <c r="L10" s="2">
+      <c r="J11" s="2">
         <v>2254.5</v>
       </c>
     </row>
@@ -3355,7 +2771,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K104"/>
   <sheetViews>
@@ -7011,11 +6427,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7175,54 +6593,25 @@
         <v>234</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>80</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>76</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11" t="s">
-        <v>234</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="18" customWidth="1"/>
+    <col min="1" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="50" customWidth="1"/>
+    <col min="4" max="9" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -7254,7 +6643,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -7283,7 +6672,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -7312,7 +6701,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -7341,7 +6730,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -7370,7 +6759,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -7399,7 +6788,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -7428,7 +6817,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -7457,7 +6846,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -7486,7 +6875,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -7515,7 +6904,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -7544,7 +6933,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -7573,7 +6962,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -7631,7 +7020,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -7660,7 +7049,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -7689,7 +7078,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -7718,7 +7107,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -7747,7 +7136,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -7776,7 +7165,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -7805,7 +7194,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -7834,7 +7223,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -7863,7 +7252,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -7892,7 +7281,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -7921,7 +7310,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -7950,7 +7339,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -7979,7 +7368,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -8008,7 +7397,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -8037,7 +7426,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -8066,7 +7455,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -8095,7 +7484,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -8124,7 +7513,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -8153,7 +7542,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -8182,7 +7571,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -8211,7 +7600,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -8240,7 +7629,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -8269,7 +7658,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -8298,7 +7687,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -8327,7 +7716,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -8356,7 +7745,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -8385,7 +7774,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>36</v>
       </c>
@@ -8414,7 +7803,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>36</v>
       </c>
@@ -8443,7 +7832,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>36</v>
       </c>
@@ -8472,7 +7861,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>36</v>
       </c>
@@ -8501,7 +7890,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>36</v>
       </c>
@@ -8530,7 +7919,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>36</v>
       </c>
@@ -8559,7 +7948,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>36</v>
       </c>
@@ -8588,7 +7977,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>36</v>
       </c>
@@ -8617,7 +8006,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>36</v>
       </c>
@@ -8646,7 +8035,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>36</v>
       </c>
@@ -8675,7 +8064,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>36</v>
       </c>
@@ -8704,7 +8093,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>36</v>
       </c>
@@ -8762,7 +8151,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>58</v>
       </c>
@@ -8849,7 +8238,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>58</v>
       </c>
@@ -8907,7 +8296,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>45</v>
       </c>
@@ -9110,7 +8499,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>45</v>
       </c>
@@ -9139,7 +8528,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>45</v>
       </c>
@@ -9168,7 +8557,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>45</v>
       </c>
@@ -9197,7 +8586,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>45</v>
       </c>
@@ -9226,7 +8615,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>45</v>
       </c>
@@ -9255,7 +8644,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>45</v>
       </c>
@@ -9284,7 +8673,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>49</v>
       </c>
@@ -9313,7 +8702,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>49</v>
       </c>
@@ -9342,7 +8731,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>49</v>
       </c>
@@ -9371,7 +8760,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>49</v>
       </c>
@@ -9400,7 +8789,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>49</v>
       </c>
@@ -9429,7 +8818,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>49</v>
       </c>
@@ -9487,7 +8876,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>49</v>
       </c>
@@ -9516,7 +8905,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>49</v>
       </c>
@@ -9545,7 +8934,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>49</v>
       </c>
@@ -9574,7 +8963,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>49</v>
       </c>
@@ -9603,7 +8992,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>49</v>
       </c>
@@ -9632,7 +9021,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>54</v>
       </c>
@@ -9922,7 +9311,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>55</v>
       </c>
@@ -9951,7 +9340,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>55</v>
       </c>
@@ -9980,7 +9369,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>55</v>
       </c>
@@ -10009,7 +9398,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>55</v>
       </c>
@@ -10038,7 +9427,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>41</v>
       </c>
@@ -10067,7 +9456,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>52</v>
       </c>
@@ -10096,7 +9485,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>52</v>
       </c>
@@ -10125,7 +9514,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>52</v>
       </c>
@@ -10154,7 +9543,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>52</v>
       </c>
@@ -10183,7 +9572,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>52</v>
       </c>
@@ -10212,7 +9601,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>52</v>
       </c>
@@ -10242,15 +9631,24 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I104" xr:uid="{00000000-0001-0000-0600-000000000000}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Evilio Polo"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10361,6 +9759,17 @@
         <v>3.992015968063872</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>377</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>59</v>
@@ -10485,4 +9894,622 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893D026F-294B-4AEA-8E08-449915C9D86F}">
+  <dimension ref="A1:S12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="11.42578125" customWidth="1"/>
+    <col min="11" max="11" width="30.7109375" customWidth="1"/>
+    <col min="12" max="18" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2">
+        <v>60</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+      <c r="D2">
+        <v>50</v>
+      </c>
+      <c r="E2">
+        <v>50</v>
+      </c>
+      <c r="F2">
+        <v>60</v>
+      </c>
+      <c r="G2">
+        <v>60</v>
+      </c>
+      <c r="H2">
+        <v>60</v>
+      </c>
+      <c r="I2" s="5">
+        <f t="shared" ref="I2:I8" si="0">SUM(B2:H2)</f>
+        <v>390</v>
+      </c>
+      <c r="K2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L2">
+        <v>40</v>
+      </c>
+      <c r="M2">
+        <v>32</v>
+      </c>
+      <c r="N2">
+        <v>32</v>
+      </c>
+      <c r="O2">
+        <v>32</v>
+      </c>
+      <c r="P2">
+        <v>40</v>
+      </c>
+      <c r="Q2">
+        <v>40</v>
+      </c>
+      <c r="R2">
+        <v>40</v>
+      </c>
+      <c r="S2" s="5">
+        <f t="shared" ref="S2:S8" si="1">SUM(L2:R2)</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3">
+        <v>60</v>
+      </c>
+      <c r="C3">
+        <v>50</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>60</v>
+      </c>
+      <c r="H3">
+        <v>60</v>
+      </c>
+      <c r="I3" s="5">
+        <f t="shared" si="0"/>
+        <v>230</v>
+      </c>
+      <c r="K3" t="s">
+        <v>71</v>
+      </c>
+      <c r="L3">
+        <v>40</v>
+      </c>
+      <c r="M3">
+        <v>32</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>40</v>
+      </c>
+      <c r="R3">
+        <v>40</v>
+      </c>
+      <c r="S3" s="5">
+        <f t="shared" si="1"/>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4">
+        <v>60</v>
+      </c>
+      <c r="C4">
+        <v>50</v>
+      </c>
+      <c r="D4">
+        <v>50</v>
+      </c>
+      <c r="E4">
+        <v>50</v>
+      </c>
+      <c r="F4">
+        <v>60</v>
+      </c>
+      <c r="G4">
+        <v>60</v>
+      </c>
+      <c r="H4">
+        <v>60</v>
+      </c>
+      <c r="I4" s="5">
+        <f t="shared" si="0"/>
+        <v>390</v>
+      </c>
+      <c r="K4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L4">
+        <v>40</v>
+      </c>
+      <c r="M4">
+        <v>32</v>
+      </c>
+      <c r="N4">
+        <v>32</v>
+      </c>
+      <c r="O4">
+        <v>32</v>
+      </c>
+      <c r="P4">
+        <v>40</v>
+      </c>
+      <c r="Q4">
+        <v>40</v>
+      </c>
+      <c r="R4">
+        <v>40</v>
+      </c>
+      <c r="S4" s="5">
+        <f t="shared" si="1"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5">
+        <v>60</v>
+      </c>
+      <c r="C5">
+        <v>50</v>
+      </c>
+      <c r="D5">
+        <v>50</v>
+      </c>
+      <c r="E5">
+        <v>50</v>
+      </c>
+      <c r="F5">
+        <v>60</v>
+      </c>
+      <c r="G5">
+        <v>60</v>
+      </c>
+      <c r="H5">
+        <v>60</v>
+      </c>
+      <c r="I5" s="5">
+        <f t="shared" si="0"/>
+        <v>390</v>
+      </c>
+      <c r="K5" t="s">
+        <v>79</v>
+      </c>
+      <c r="L5">
+        <v>40</v>
+      </c>
+      <c r="M5">
+        <v>32</v>
+      </c>
+      <c r="N5">
+        <v>32</v>
+      </c>
+      <c r="O5">
+        <v>32</v>
+      </c>
+      <c r="P5">
+        <v>40</v>
+      </c>
+      <c r="Q5">
+        <v>40</v>
+      </c>
+      <c r="R5">
+        <v>40</v>
+      </c>
+      <c r="S5" s="5">
+        <f t="shared" si="1"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6">
+        <v>60</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
+      </c>
+      <c r="D6">
+        <v>50</v>
+      </c>
+      <c r="E6">
+        <v>50</v>
+      </c>
+      <c r="F6">
+        <v>60</v>
+      </c>
+      <c r="G6">
+        <v>60</v>
+      </c>
+      <c r="H6">
+        <v>60</v>
+      </c>
+      <c r="I6" s="5">
+        <f t="shared" si="0"/>
+        <v>390</v>
+      </c>
+      <c r="K6" t="s">
+        <v>83</v>
+      </c>
+      <c r="L6">
+        <v>40</v>
+      </c>
+      <c r="M6">
+        <v>32</v>
+      </c>
+      <c r="N6">
+        <v>32</v>
+      </c>
+      <c r="O6">
+        <v>32</v>
+      </c>
+      <c r="P6">
+        <v>40</v>
+      </c>
+      <c r="Q6">
+        <v>40</v>
+      </c>
+      <c r="R6">
+        <v>40</v>
+      </c>
+      <c r="S6" s="5">
+        <f t="shared" si="1"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7">
+        <v>30</v>
+      </c>
+      <c r="C7">
+        <v>30</v>
+      </c>
+      <c r="D7">
+        <v>30</v>
+      </c>
+      <c r="E7">
+        <v>30</v>
+      </c>
+      <c r="F7">
+        <v>30</v>
+      </c>
+      <c r="G7">
+        <v>30</v>
+      </c>
+      <c r="H7">
+        <v>30</v>
+      </c>
+      <c r="I7" s="5">
+        <f t="shared" si="0"/>
+        <v>210</v>
+      </c>
+      <c r="K7" t="s">
+        <v>81</v>
+      </c>
+      <c r="L7">
+        <v>20</v>
+      </c>
+      <c r="M7">
+        <v>20</v>
+      </c>
+      <c r="N7">
+        <v>20</v>
+      </c>
+      <c r="O7">
+        <v>20</v>
+      </c>
+      <c r="P7">
+        <v>20</v>
+      </c>
+      <c r="Q7">
+        <v>20</v>
+      </c>
+      <c r="R7">
+        <v>20</v>
+      </c>
+      <c r="S7" s="5">
+        <f t="shared" si="1"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8">
+        <v>60</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>50</v>
+      </c>
+      <c r="E8">
+        <v>50</v>
+      </c>
+      <c r="F8">
+        <v>60</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5">
+        <f t="shared" si="0"/>
+        <v>220</v>
+      </c>
+      <c r="K8" t="s">
+        <v>82</v>
+      </c>
+      <c r="L8">
+        <v>40</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>32</v>
+      </c>
+      <c r="O8">
+        <v>32</v>
+      </c>
+      <c r="P8">
+        <v>40</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8" s="5">
+        <f t="shared" si="1"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9">
+        <v>60</v>
+      </c>
+      <c r="C9">
+        <v>60</v>
+      </c>
+      <c r="D9">
+        <v>60</v>
+      </c>
+      <c r="E9">
+        <v>60</v>
+      </c>
+      <c r="F9">
+        <v>60</v>
+      </c>
+      <c r="G9">
+        <v>60</v>
+      </c>
+      <c r="H9">
+        <v>60</v>
+      </c>
+      <c r="I9" s="5">
+        <f>SUM(B9:H9)</f>
+        <v>420</v>
+      </c>
+      <c r="K9" t="s">
+        <v>68</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>40</v>
+      </c>
+      <c r="N9">
+        <v>40</v>
+      </c>
+      <c r="O9">
+        <v>40</v>
+      </c>
+      <c r="P9">
+        <v>40</v>
+      </c>
+      <c r="Q9">
+        <v>40</v>
+      </c>
+      <c r="R9">
+        <v>40</v>
+      </c>
+      <c r="S9" s="5">
+        <f>SUM(M9:R9)</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="B10">
+        <f>SUM(B2:B9)</f>
+        <v>450</v>
+      </c>
+      <c r="C10">
+        <f>SUM(C2:C9)</f>
+        <v>340</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ref="C10:H10" si="2">SUM(D2:D8)</f>
+        <v>280</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>280</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="2"/>
+        <v>330</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>330</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>330</v>
+      </c>
+      <c r="I10" s="5">
+        <f>SUM(B10:H10)</f>
+        <v>2340</v>
+      </c>
+      <c r="J10" s="5"/>
+      <c r="K10" t="s">
+        <v>372</v>
+      </c>
+      <c r="L10">
+        <f>SUM(L2:L8)</f>
+        <v>260</v>
+      </c>
+      <c r="M10">
+        <f t="shared" ref="M10" si="3">SUM(M2:M8)</f>
+        <v>180</v>
+      </c>
+      <c r="N10">
+        <f t="shared" ref="N10" si="4">SUM(N2:N8)</f>
+        <v>180</v>
+      </c>
+      <c r="O10">
+        <f t="shared" ref="O10" si="5">SUM(O2:O8)</f>
+        <v>180</v>
+      </c>
+      <c r="P10">
+        <f t="shared" ref="P10" si="6">SUM(P2:P8)</f>
+        <v>220</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" ref="Q10" si="7">SUM(Q2:Q8)</f>
+        <v>220</v>
+      </c>
+      <c r="R10">
+        <f t="shared" ref="R10" si="8">SUM(R2:R8)</f>
+        <v>220</v>
+      </c>
+      <c r="S10" s="5">
+        <f>SUM(L10:R10)</f>
+        <v>1460</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K12" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>